<commit_message>
Fertige Exceltabelle ohne Magic Charts
</commit_message>
<xml_diff>
--- a/Ausgabe/Belege.xlsx
+++ b/Ausgabe/Belege.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <x:si>
     <x:t>Tankstelle</x:t>
   </x:si>
@@ -61,13 +61,16 @@
     <x:t>79.207</x:t>
   </x:si>
   <x:si>
-    <x:t>PBSN23</x:t>
+    <x:t>0.74</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PBSN23E</x:t>
   </x:si>
   <x:si>
     <x:t>Nein</x:t>
   </x:si>
   <x:si>
-    <x:t>49,17 €</x:t>
+    <x:t>58.91 EUR</x:t>
   </x:si>
   <x:si>
     <x:t>Aral</x:t>
@@ -79,16 +82,16 @@
     <x:t>Super</x:t>
   </x:si>
   <x:si>
+    <x:t>42,63</x:t>
+  </x:si>
+  <x:si>
     <x:t>1,729</x:t>
   </x:si>
   <x:si>
     <x:t>16488</x:t>
   </x:si>
   <x:si>
-    <x:t>PBSN23E</x:t>
-  </x:si>
-  <x:si>
-    <x:t>73,71 EUR</x:t>
+    <x:t>73.71 EUR</x:t>
   </x:si>
   <x:si>
     <x:t>HEM</x:t>
@@ -106,7 +109,7 @@
     <x:t>18243</x:t>
   </x:si>
   <x:si>
-    <x:t>70,55 EUR</x:t>
+    <x:t>70.55 EUR</x:t>
   </x:si>
   <x:si>
     <x:t>27.04.2025</x:t>
@@ -115,13 +118,16 @@
     <x:t>Super E10</x:t>
   </x:si>
   <x:si>
+    <x:t>43,84</x:t>
+  </x:si>
+  <x:si>
     <x:t>1,669</x:t>
   </x:si>
   <x:si>
     <x:t>17704</x:t>
   </x:si>
   <x:si>
-    <x:t>73,17 EUR</x:t>
+    <x:t>73.17 EUR</x:t>
   </x:si>
   <x:si>
     <x:t>Total</x:t>
@@ -136,7 +142,7 @@
     <x:t>Ja</x:t>
   </x:si>
   <x:si>
-    <x:t>17,50 EUR</x:t>
+    <x:t>17.50 EUR</x:t>
   </x:si>
   <x:si>
     <x:t>15.04.2025</x:t>
@@ -151,7 +157,7 @@
     <x:t>16997</x:t>
   </x:si>
   <x:si>
-    <x:t>61,75 EUR</x:t>
+    <x:t>61.75 EUR</x:t>
   </x:si>
   <x:si>
     <x:t>29.03.2025</x:t>
@@ -163,7 +169,7 @@
     <x:t>15787</x:t>
   </x:si>
   <x:si>
-    <x:t>73,32 EUR</x:t>
+    <x:t>73.32 EUR</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -568,173 +574,182 @@
       <x:c r="E2" s="0" t="s">
         <x:v>14</x:v>
       </x:c>
+      <x:c r="G2" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
       <x:c r="I2" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="J2" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="K2" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:11">
       <x:c r="A3" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F3" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="H3" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="I3" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="J3" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="K3" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:11">
       <x:c r="A4" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="F4" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="H4" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="I4" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="J4" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="K4" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:11">
       <x:c r="A5" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>34</x:v>
       </x:c>
       <x:c r="F5" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="H5" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="I5" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="J5" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="K5" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>37</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:11">
       <x:c r="A6" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="H6" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="I6" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="J6" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="K6" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>42</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:11">
       <x:c r="A7" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="F7" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="H7" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="I7" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="J7" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="K7" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>47</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:11">
       <x:c r="A8" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="F8" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="H8" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="I8" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="J8" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="K8" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>51</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>